<commit_message>
Adiciona análise ENADE com gráficos e dados do Excel
</commit_message>
<xml_diff>
--- a/dadosenade.xlsx
+++ b/dadosenade.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gpslg\Desktop\enade-dados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9F6834E28CA88343/Documentos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15BE415E-A8CF-4717-8529-3CD56F717854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{8882FC0B-4751-4E52-80C2-62012BB92708}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{70EED58D-BB6C-489B-A79F-930FE9090737}"/>
   <bookViews>
-    <workbookView xWindow="3360" yWindow="2100" windowWidth="14400" windowHeight="7290" xr2:uid="{8D3C7461-333D-4B53-ADA6-D1F8F66C3259}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8D3C7461-333D-4B53-ADA6-D1F8F66C3259}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -129,8 +129,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -158,8 +166,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -496,23 +505,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F5F245B-9FEF-44A6-B534-930D97288894}">
   <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9.453125" customWidth="1"/>
-    <col min="3" max="3" width="12.7265625" customWidth="1"/>
-    <col min="5" max="5" width="12.1796875" customWidth="1"/>
-    <col min="6" max="6" width="16.7265625" customWidth="1"/>
-    <col min="7" max="7" width="10.7265625" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" customWidth="1"/>
+    <col min="3" max="3" width="12.77734375" customWidth="1"/>
+    <col min="5" max="5" width="12.21875" customWidth="1"/>
+    <col min="6" max="6" width="16.77734375" customWidth="1"/>
+    <col min="7" max="7" width="10.77734375" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
-    <col min="9" max="9" width="9.1796875" customWidth="1"/>
-    <col min="10" max="10" width="14.26953125" customWidth="1"/>
+    <col min="9" max="9" width="9.21875" customWidth="1"/>
+    <col min="10" max="10" width="14.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -544,7 +553,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2008</v>
       </c>
@@ -564,7 +573,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2011</v>
       </c>
@@ -584,7 +593,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2014</v>
       </c>
@@ -604,7 +613,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2017</v>
       </c>
@@ -624,7 +633,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2019</v>
       </c>
@@ -644,7 +653,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2023</v>
       </c>
@@ -664,7 +673,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2026</v>
       </c>
@@ -696,7 +705,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2008</v>
       </c>
@@ -716,7 +725,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2014</v>
       </c>
@@ -736,7 +745,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2017</v>
       </c>
@@ -756,7 +765,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2019</v>
       </c>
@@ -776,7 +785,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2023</v>
       </c>
@@ -796,7 +805,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2026</v>
       </c>
@@ -828,7 +837,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2014</v>
       </c>
@@ -848,7 +857,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2017</v>
       </c>
@@ -868,7 +877,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2019</v>
       </c>
@@ -888,7 +897,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2023</v>
       </c>
@@ -908,7 +917,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2026</v>
       </c>
@@ -940,7 +949,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2011</v>
       </c>
@@ -960,7 +969,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2014</v>
       </c>
@@ -980,7 +989,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2017</v>
       </c>
@@ -1000,7 +1009,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2019</v>
       </c>
@@ -1020,7 +1029,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2023</v>
       </c>
@@ -1040,7 +1049,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2026</v>
       </c>
@@ -1072,7 +1081,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>2014</v>
       </c>
@@ -1092,7 +1101,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>2017</v>
       </c>
@@ -1112,7 +1121,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>2019</v>
       </c>
@@ -1132,7 +1141,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>2023</v>
       </c>
@@ -1152,7 +1161,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>2026</v>
       </c>
@@ -1184,7 +1193,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>2011</v>
       </c>
@@ -1204,7 +1213,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>2014</v>
       </c>
@@ -1224,7 +1233,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>2017</v>
       </c>
@@ -1244,7 +1253,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>2019</v>
       </c>
@@ -1264,7 +1273,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>2023</v>
       </c>
@@ -1284,7 +1293,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>2026</v>
       </c>
@@ -1316,7 +1325,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>2017</v>
       </c>
@@ -1336,7 +1345,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>2019</v>
       </c>
@@ -1356,7 +1365,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>2023</v>
       </c>
@@ -1376,10 +1385,13 @@
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>2026</v>
       </c>
+      <c r="B40">
+        <v>3</v>
+      </c>
       <c r="C40" t="s">
         <v>16</v>
       </c>
@@ -1392,8 +1404,20 @@
       <c r="F40" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="G40">
+        <v>0.17857139999999999</v>
+      </c>
+      <c r="H40">
+        <v>-357.32142900000002</v>
+      </c>
+      <c r="I40">
+        <v>4.4642860000000004</v>
+      </c>
+      <c r="J40">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>2014</v>
       </c>
@@ -1413,7 +1437,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>2017</v>
       </c>
@@ -1433,7 +1457,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>2019</v>
       </c>
@@ -1453,7 +1477,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>2023</v>
       </c>
@@ -1473,7 +1497,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>2026</v>
       </c>
@@ -1505,7 +1529,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>2014</v>
       </c>
@@ -1525,7 +1549,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>2017</v>
       </c>
@@ -1545,7 +1569,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>2019</v>
       </c>
@@ -1565,7 +1589,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>2023</v>
       </c>
@@ -1585,10 +1609,13 @@
         <v>26</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>2026</v>
       </c>
+      <c r="B50">
+        <v>4</v>
+      </c>
       <c r="C50" t="s">
         <v>17</v>
       </c>
@@ -1614,7 +1641,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>2005</v>
       </c>
@@ -1634,7 +1661,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>2008</v>
       </c>
@@ -1654,7 +1681,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>2011</v>
       </c>
@@ -1674,7 +1701,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>2014</v>
       </c>
@@ -1694,7 +1721,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>2017</v>
       </c>
@@ -1714,7 +1741,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>2019</v>
       </c>
@@ -1734,7 +1761,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>2023</v>
       </c>
@@ -1754,10 +1781,13 @@
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>2026</v>
       </c>
+      <c r="B58">
+        <v>3</v>
+      </c>
       <c r="C58" t="s">
         <v>18</v>
       </c>
@@ -1783,7 +1813,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>2005</v>
       </c>
@@ -1803,7 +1833,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>2008</v>
       </c>
@@ -1823,7 +1853,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>2011</v>
       </c>
@@ -1843,7 +1873,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>2014</v>
       </c>
@@ -1863,7 +1893,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>2017</v>
       </c>
@@ -1882,8 +1912,9 @@
       <c r="F63" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="G63" s="1"/>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>2019</v>
       </c>
@@ -1903,7 +1934,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>2023</v>
       </c>
@@ -1923,7 +1954,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>2026</v>
       </c>
@@ -1943,16 +1974,16 @@
         <v>28</v>
       </c>
       <c r="G66">
-        <f>SLOPE(B59:B65,A59:A65)</f>
-        <v>-2.1352313167259791E-2</v>
+        <f>SLOPE(B2:B66,A2:A66)</f>
+        <v>2.3701885817618205E-2</v>
       </c>
       <c r="H66">
-        <f>INTERCEPT(B59:B65,A59:A65)</f>
-        <v>44.857651245551608</v>
+        <f>INTERCEPT(B2:B66,A2:A66)</f>
+        <v>-44.738827176440232</v>
       </c>
       <c r="I66">
-        <f>FORECAST(2026,B59:B65,A59:A65)</f>
-        <v>1.597864768683273</v>
+        <f>FORECAST(2026,B2:B66,A2:A66)</f>
+        <v>3.2811934900542497</v>
       </c>
       <c r="J66">
         <v>2</v>
@@ -1960,5 +1991,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>